<commit_message>
Add Inflation_contributions_graph_data.XLSX, Waterfall_graph_data.XLSX, trimmed_graph_data.XLSX, MEGA_DATA_DOWNLOAD.xlsx, SUMMARY_EXPORT_DATA_DOWNLOAD.xlsx and EXPORT_DATA_DOWNLOAD_ALL.xlsx
</commit_message>
<xml_diff>
--- a/EXPORT_DATA_DOWNLOAD_ALL.xlsx
+++ b/EXPORT_DATA_DOWNLOAD_ALL.xlsx
@@ -15869,7 +15869,7 @@
         <v>-27.69</v>
       </c>
       <c r="AM98" t="n">
-        <v>94.05</v>
+        <v>11.01</v>
       </c>
       <c r="AN98" t="n">
         <v>71.01</v>
@@ -15905,7 +15905,7 @@
         <v>-4.01</v>
       </c>
       <c r="AY98" t="n">
-        <v>22.31</v>
+        <v>22.01</v>
       </c>
     </row>
     <row r="99">
@@ -16068,154 +16068,154 @@
         <v>45352</v>
       </c>
       <c r="B100" t="n">
-        <v>6.98</v>
+        <v>7.25</v>
       </c>
       <c r="C100" t="n">
-        <v>31</v>
+        <v>87.23</v>
       </c>
       <c r="D100" t="n">
-        <v>39.91</v>
+        <v>39.83</v>
       </c>
       <c r="E100" t="n">
-        <v>-33.13</v>
+        <v>-30.54</v>
       </c>
       <c r="F100" t="n">
-        <v>634.25</v>
+        <v>874.84</v>
       </c>
       <c r="G100" t="n">
-        <v>128.97</v>
+        <v>140.2</v>
       </c>
       <c r="H100" t="n">
-        <v>-23.22</v>
+        <v>-16.58</v>
       </c>
       <c r="I100" t="n">
-        <v>4.83</v>
+        <v>14.18</v>
       </c>
       <c r="J100" t="n">
-        <v>-4.75</v>
+        <v>-1.68</v>
       </c>
       <c r="K100" t="n">
-        <v>-60.82</v>
+        <v>-61.03</v>
       </c>
       <c r="L100" t="n">
-        <v>-5.92</v>
+        <v>-6.55</v>
       </c>
       <c r="M100" t="n">
-        <v>-26.85</v>
+        <v>-26.12</v>
       </c>
       <c r="N100" t="n">
-        <v>-2.65</v>
+        <v>-1.68</v>
       </c>
       <c r="O100" t="n">
-        <v>15.22</v>
+        <v>24.12</v>
       </c>
       <c r="P100" t="n">
-        <v>-47.57</v>
+        <v>-48.06</v>
       </c>
       <c r="Q100" t="n">
-        <v>-18.47</v>
+        <v>-18.14</v>
       </c>
       <c r="R100" t="n">
-        <v>142.81</v>
+        <v>145.13</v>
       </c>
       <c r="S100" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="T100" t="n">
-        <v>-13.06</v>
+        <v>-13.24</v>
       </c>
       <c r="U100" t="n">
         <v>-18.81</v>
       </c>
       <c r="V100" t="n">
-        <v>-22.01</v>
+        <v>-9.16</v>
       </c>
       <c r="W100" t="n">
-        <v>6.54</v>
+        <v>29.63</v>
       </c>
       <c r="X100" t="n">
         <v>-44.15</v>
       </c>
       <c r="Y100" t="n">
-        <v>-35.04</v>
+        <v>-34.41</v>
       </c>
       <c r="Z100" t="n">
-        <v>-8</v>
+        <v>-3.14</v>
       </c>
       <c r="AA100" t="n">
-        <v>-41</v>
+        <v>-44.02</v>
       </c>
       <c r="AB100" t="n">
-        <v>16.07</v>
+        <v>20.11</v>
       </c>
       <c r="AC100" t="n">
-        <v>29.3</v>
+        <v>28.75</v>
       </c>
       <c r="AD100" t="n">
-        <v>116.1</v>
+        <v>150.88</v>
       </c>
       <c r="AE100" t="n">
-        <v>-10.31</v>
+        <v>-10.5</v>
       </c>
       <c r="AF100" t="n">
-        <v>-63.66</v>
+        <v>-65.09</v>
       </c>
       <c r="AG100" t="n">
-        <v>-20.4</v>
+        <v>-19.88</v>
       </c>
       <c r="AH100" t="n">
-        <v>-82.1</v>
+        <v>-83.53</v>
       </c>
       <c r="AI100" t="n">
-        <v>-38.2</v>
+        <v>-38.12</v>
       </c>
       <c r="AJ100" t="n">
         <v>54.66</v>
       </c>
       <c r="AK100" t="n">
-        <v>-0.49</v>
+        <v>-2.14</v>
       </c>
       <c r="AL100" t="n">
-        <v>-3.5</v>
+        <v>-2.24</v>
       </c>
       <c r="AM100" t="n">
         <v>-5.87</v>
       </c>
       <c r="AN100" t="n">
-        <v>17.31</v>
+        <v>16.44</v>
       </c>
       <c r="AO100" t="n">
-        <v>-3.53</v>
+        <v>-2.61</v>
       </c>
       <c r="AP100" t="n">
         <v>-53.06</v>
       </c>
       <c r="AQ100" t="n">
-        <v>-7.38</v>
+        <v>-10.26</v>
       </c>
       <c r="AR100" t="n">
         <v>2.05</v>
       </c>
       <c r="AS100" t="n">
-        <v>-8.9</v>
+        <v>-8.63</v>
       </c>
       <c r="AT100" t="n">
-        <v>5.29</v>
+        <v>7.57</v>
       </c>
       <c r="AU100" t="n">
-        <v>0.16</v>
+        <v>1.22</v>
       </c>
       <c r="AV100" t="n">
-        <v>-46.79</v>
+        <v>-49.11</v>
       </c>
       <c r="AW100" t="n">
-        <v>56.29</v>
+        <v>7.14</v>
       </c>
       <c r="AX100" t="n">
-        <v>-4.32</v>
+        <v>-5.48</v>
       </c>
       <c r="AY100" t="n">
-        <v>-0.45</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="101">
@@ -16843,16 +16843,16 @@
         <v>45505</v>
       </c>
       <c r="B105" t="n">
-        <v>-23.25</v>
+        <v>-22.11</v>
       </c>
       <c r="C105" t="n">
         <v>6.91</v>
       </c>
       <c r="D105" t="n">
-        <v>-21.49</v>
+        <v>-21.77</v>
       </c>
       <c r="E105" t="n">
-        <v>-4.24</v>
+        <v>-3.45</v>
       </c>
       <c r="F105" t="n">
         <v>-58.04</v>
@@ -16867,34 +16867,34 @@
         <v>0.96</v>
       </c>
       <c r="J105" t="n">
-        <v>12.72</v>
+        <v>16.27</v>
       </c>
       <c r="K105" t="n">
-        <v>-54.62</v>
+        <v>-54.93</v>
       </c>
       <c r="L105" t="n">
-        <v>24.14</v>
+        <v>24.15</v>
       </c>
       <c r="M105" t="n">
-        <v>-11.42</v>
+        <v>-15.76</v>
       </c>
       <c r="N105" t="n">
-        <v>13.43</v>
+        <v>17.24</v>
       </c>
       <c r="O105" t="n">
-        <v>60.57</v>
+        <v>59.62</v>
       </c>
       <c r="P105" t="n">
-        <v>-38.62</v>
+        <v>-38.86</v>
       </c>
       <c r="Q105" t="n">
-        <v>-12.78</v>
+        <v>-10.13</v>
       </c>
       <c r="R105" t="n">
-        <v>16.55</v>
+        <v>16.63</v>
       </c>
       <c r="S105" t="n">
-        <v>220.55</v>
+        <v>217.84</v>
       </c>
       <c r="T105" t="n">
         <v>48.72</v>
@@ -16903,7 +16903,7 @@
         <v>-18.17</v>
       </c>
       <c r="V105" t="n">
-        <v>5.09</v>
+        <v>4.13</v>
       </c>
       <c r="W105" t="n">
         <v>-46.98</v>
@@ -16912,16 +16912,16 @@
         <v>9.15</v>
       </c>
       <c r="Y105" t="n">
-        <v>17.77</v>
+        <v>11.14</v>
       </c>
       <c r="Z105" t="n">
-        <v>-2.5</v>
+        <v>-1.84</v>
       </c>
       <c r="AA105" t="n">
-        <v>17.73</v>
+        <v>17.17</v>
       </c>
       <c r="AB105" t="n">
-        <v>-15.58</v>
+        <v>-14.58</v>
       </c>
       <c r="AC105" t="n">
         <v>1.62</v>
@@ -16930,19 +16930,19 @@
         <v>79.24</v>
       </c>
       <c r="AE105" t="n">
-        <v>4.42</v>
+        <v>4.05</v>
       </c>
       <c r="AF105" t="n">
         <v>-27.67</v>
       </c>
       <c r="AG105" t="n">
-        <v>-30.14</v>
+        <v>-29.95</v>
       </c>
       <c r="AH105" t="n">
-        <v>-32.56</v>
+        <v>-29.38</v>
       </c>
       <c r="AI105" t="n">
-        <v>4.99</v>
+        <v>4.33</v>
       </c>
       <c r="AJ105" t="n">
         <v>106.79</v>
@@ -16951,16 +16951,16 @@
         <v>-14.83</v>
       </c>
       <c r="AL105" t="n">
-        <v>8.53</v>
+        <v>16.5</v>
       </c>
       <c r="AM105" t="n">
         <v>-3.32</v>
       </c>
       <c r="AN105" t="n">
-        <v>57.63</v>
+        <v>61.28</v>
       </c>
       <c r="AO105" t="n">
-        <v>13.57</v>
+        <v>6.93</v>
       </c>
       <c r="AP105" t="n">
         <v>98.86</v>
@@ -16978,19 +16978,174 @@
         <v>-5.74</v>
       </c>
       <c r="AU105" t="n">
-        <v>-1.32</v>
+        <v>-2.41</v>
       </c>
       <c r="AV105" t="n">
         <v>156.28</v>
       </c>
       <c r="AW105" t="n">
-        <v>12.02</v>
+        <v>-9.98</v>
       </c>
       <c r="AX105" t="n">
-        <v>2.63</v>
+        <v>2.49</v>
       </c>
       <c r="AY105" t="n">
-        <v>7.49</v>
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B106" t="n">
+        <v>33.69</v>
+      </c>
+      <c r="C106" t="n">
+        <v>81.67</v>
+      </c>
+      <c r="D106" t="n">
+        <v>41.98</v>
+      </c>
+      <c r="E106" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="F106" t="n">
+        <v>-8.96</v>
+      </c>
+      <c r="G106" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="H106" t="n">
+        <v>16.66</v>
+      </c>
+      <c r="I106" t="n">
+        <v>-7.11</v>
+      </c>
+      <c r="J106" t="n">
+        <v>-5.04</v>
+      </c>
+      <c r="K106" t="n">
+        <v>-63.97</v>
+      </c>
+      <c r="L106" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="M106" t="n">
+        <v>-13.4</v>
+      </c>
+      <c r="N106" t="n">
+        <v>-35.64</v>
+      </c>
+      <c r="O106" t="n">
+        <v>513.42</v>
+      </c>
+      <c r="P106" t="n">
+        <v>-8.1</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>-17.14</v>
+      </c>
+      <c r="R106" t="n">
+        <v>-34.78</v>
+      </c>
+      <c r="S106" t="n">
+        <v>330.52</v>
+      </c>
+      <c r="T106" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="U106" t="n">
+        <v>-26.77</v>
+      </c>
+      <c r="V106" t="n">
+        <v>69.89</v>
+      </c>
+      <c r="W106" t="n">
+        <v>-11.75</v>
+      </c>
+      <c r="X106" t="n">
+        <v>44.84</v>
+      </c>
+      <c r="Y106" t="n">
+        <v>-35.66</v>
+      </c>
+      <c r="Z106" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA106" t="n">
+        <v>-23.26</v>
+      </c>
+      <c r="AB106" t="n">
+        <v>26.11</v>
+      </c>
+      <c r="AC106" t="n">
+        <v>64.86</v>
+      </c>
+      <c r="AD106" t="n">
+        <v>53.73</v>
+      </c>
+      <c r="AE106" t="n">
+        <v>51.99</v>
+      </c>
+      <c r="AF106" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="AG106" t="n">
+        <v>-6.79</v>
+      </c>
+      <c r="AH106" t="n">
+        <v>-32.46</v>
+      </c>
+      <c r="AI106" t="n">
+        <v>23.74</v>
+      </c>
+      <c r="AJ106" t="n">
+        <v>118.45</v>
+      </c>
+      <c r="AK106" t="n">
+        <v>-55.67</v>
+      </c>
+      <c r="AL106" t="n">
+        <v>43.64</v>
+      </c>
+      <c r="AM106" t="n">
+        <v>56.1</v>
+      </c>
+      <c r="AN106" t="n">
+        <v>-9.58</v>
+      </c>
+      <c r="AO106" t="n">
+        <v>15.26</v>
+      </c>
+      <c r="AP106" t="n">
+        <v>-24.83</v>
+      </c>
+      <c r="AQ106" t="n">
+        <v>-2.37</v>
+      </c>
+      <c r="AR106" t="n">
+        <v>86.01</v>
+      </c>
+      <c r="AS106" t="n">
+        <v>64.19</v>
+      </c>
+      <c r="AT106" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="AU106" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="AV106" t="n">
+        <v>80.86</v>
+      </c>
+      <c r="AW106" t="n">
+        <v>30.6</v>
+      </c>
+      <c r="AX106" t="n">
+        <v>25.15</v>
+      </c>
+      <c r="AY106" t="n">
+        <v>40.35</v>
       </c>
     </row>
   </sheetData>
@@ -32158,7 +32313,7 @@
         <v>-0.17</v>
       </c>
       <c r="AM98" t="n">
-        <v>0.34</v>
+        <v>0.04</v>
       </c>
       <c r="AN98" t="n">
         <v>0.04</v>
@@ -32194,7 +32349,7 @@
         <v>-0.14</v>
       </c>
       <c r="AY98" t="n">
-        <v>22.31</v>
+        <v>22.01</v>
       </c>
     </row>
     <row r="99">
@@ -32360,25 +32515,25 @@
         <v>0.02</v>
       </c>
       <c r="C100" t="n">
-        <v>0.13</v>
+        <v>0.36</v>
       </c>
       <c r="D100" t="n">
-        <v>2.8</v>
+        <v>2.79</v>
       </c>
       <c r="E100" t="n">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
       <c r="F100" t="n">
-        <v>0.61</v>
+        <v>0.84</v>
       </c>
       <c r="G100" t="n">
-        <v>2.69</v>
+        <v>2.93</v>
       </c>
       <c r="H100" t="n">
-        <v>-0.67</v>
+        <v>-0.48</v>
       </c>
       <c r="I100" t="n">
-        <v>0.24</v>
+        <v>0.7</v>
       </c>
       <c r="J100" t="n">
         <v>0</v>
@@ -32387,7 +32542,7 @@
         <v>-0.4</v>
       </c>
       <c r="L100" t="n">
-        <v>-0.63</v>
+        <v>-0.7</v>
       </c>
       <c r="M100" t="n">
         <v>-0.1</v>
@@ -32396,13 +32551,13 @@
         <v>0</v>
       </c>
       <c r="O100" t="n">
-        <v>0.2</v>
+        <v>0.31</v>
       </c>
       <c r="P100" t="n">
         <v>-0.07</v>
       </c>
       <c r="Q100" t="n">
-        <v>-0.57</v>
+        <v>-0.56</v>
       </c>
       <c r="R100" t="n">
         <v>0.23</v>
@@ -32417,10 +32572,10 @@
         <v>-0.04</v>
       </c>
       <c r="V100" t="n">
-        <v>-0.87</v>
+        <v>-0.36</v>
       </c>
       <c r="W100" t="n">
-        <v>0.13</v>
+        <v>0.59</v>
       </c>
       <c r="X100" t="n">
         <v>-0.26</v>
@@ -32438,13 +32593,13 @@
         <v>0</v>
       </c>
       <c r="AC100" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="AD100" t="n">
-        <v>0.78</v>
+        <v>1.02</v>
       </c>
       <c r="AE100" t="n">
-        <v>-0.71</v>
+        <v>-0.73</v>
       </c>
       <c r="AF100" t="n">
         <v>-0.16</v>
@@ -32453,7 +32608,7 @@
         <v>-0.16</v>
       </c>
       <c r="AH100" t="n">
-        <v>-1.28</v>
+        <v>-1.3</v>
       </c>
       <c r="AI100" t="n">
         <v>-0.1</v>
@@ -32462,10 +32617,10 @@
         <v>0.1</v>
       </c>
       <c r="AK100" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="AL100" t="n">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="AM100" t="n">
         <v>-0.03</v>
@@ -32480,31 +32635,31 @@
         <v>-0.14</v>
       </c>
       <c r="AQ100" t="n">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="AR100" t="n">
         <v>0</v>
       </c>
       <c r="AS100" t="n">
-        <v>-2.67</v>
+        <v>-2.58</v>
       </c>
       <c r="AT100" t="n">
-        <v>0.48</v>
+        <v>0.68</v>
       </c>
       <c r="AU100" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AV100" t="n">
         <v>-0.11</v>
       </c>
       <c r="AW100" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="AX100" t="n">
-        <v>-0.12</v>
+        <v>-0.16</v>
       </c>
       <c r="AY100" t="n">
-        <v>-0.45</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="101">
@@ -33138,7 +33293,7 @@
         <v>0.03</v>
       </c>
       <c r="D105" t="n">
-        <v>-2.49</v>
+        <v>-2.52</v>
       </c>
       <c r="E105" t="n">
         <v>-0.01</v>
@@ -33165,19 +33320,19 @@
         <v>1.84</v>
       </c>
       <c r="M105" t="n">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="N105" t="n">
         <v>0</v>
       </c>
       <c r="O105" t="n">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="P105" t="n">
         <v>-0.06</v>
       </c>
       <c r="Q105" t="n">
-        <v>-0.46</v>
+        <v>-0.37</v>
       </c>
       <c r="R105" t="n">
         <v>0.03</v>
@@ -33192,7 +33347,7 @@
         <v>-0.04</v>
       </c>
       <c r="V105" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="W105" t="n">
         <v>-1.12</v>
@@ -33201,7 +33356,7 @@
         <v>0.03</v>
       </c>
       <c r="Y105" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="Z105" t="n">
         <v>0</v>
@@ -33219,7 +33374,7 @@
         <v>0.5</v>
       </c>
       <c r="AE105" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="AF105" t="n">
         <v>-0.05</v>
@@ -33240,7 +33395,7 @@
         <v>-0.06</v>
       </c>
       <c r="AL105" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="AM105" t="n">
         <v>-0.01</v>
@@ -33249,7 +33404,7 @@
         <v>0.02</v>
       </c>
       <c r="AO105" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AP105" t="n">
         <v>0.12</v>
@@ -33267,19 +33422,174 @@
         <v>-0.46</v>
       </c>
       <c r="AU105" t="n">
-        <v>-0.03</v>
+        <v>-0.06</v>
       </c>
       <c r="AV105" t="n">
         <v>0.2</v>
       </c>
       <c r="AW105" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="AX105" t="n">
         <v>0.08</v>
       </c>
       <c r="AY105" t="n">
-        <v>7.49</v>
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D106" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I106" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="L106" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="M106" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="N106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="O106" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="P106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="R106" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="S106" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="T106" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="U106" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="V106" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="W106" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="X106" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Y106" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="Z106" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AA106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AB106" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC106" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="AD106" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AE106" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="AF106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG106" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="AH106" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="AI106" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AJ106" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="AK106" t="n">
+        <v>-0.37</v>
+      </c>
+      <c r="AL106" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="AM106" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="AN106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AO106" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AP106" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="AQ106" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AR106" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AS106" t="n">
+        <v>17.15</v>
+      </c>
+      <c r="AT106" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="AU106" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AV106" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AW106" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AX106" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="AY106" t="n">
+        <v>40.35</v>
       </c>
     </row>
   </sheetData>
@@ -53676,7 +53986,7 @@
         <v>54.24</v>
       </c>
       <c r="AU110" t="n">
-        <v>118.47</v>
+        <v>60.85</v>
       </c>
       <c r="AV110" t="n">
         <v>-12.88</v>
@@ -53941,199 +54251,199 @@
         <v>45352</v>
       </c>
       <c r="B112" t="n">
-        <v>53.32</v>
+        <v>54.1</v>
       </c>
       <c r="C112" t="n">
-        <v>-4.75</v>
+        <v>-4.98</v>
       </c>
       <c r="D112" t="n">
-        <v>-25.1</v>
+        <v>-24.77</v>
       </c>
       <c r="E112" t="n">
-        <v>-5.71</v>
+        <v>-6.63</v>
       </c>
       <c r="F112" t="n">
-        <v>-7.74</v>
+        <v>-7.15</v>
       </c>
       <c r="G112" t="n">
-        <v>11.58</v>
+        <v>12.9</v>
       </c>
       <c r="H112" t="n">
-        <v>-1.24</v>
+        <v>-3.23</v>
       </c>
       <c r="I112" t="n">
-        <v>-17.36</v>
+        <v>-20.45</v>
       </c>
       <c r="J112" t="n">
-        <v>-7.82</v>
+        <v>-7.49</v>
       </c>
       <c r="K112" t="n">
-        <v>-8.74</v>
+        <v>-9.19</v>
       </c>
       <c r="L112" t="n">
-        <v>19.8</v>
+        <v>19.38</v>
       </c>
       <c r="M112" t="n">
         <v>-48.46</v>
       </c>
       <c r="N112" t="n">
-        <v>2.44</v>
+        <v>2.31</v>
       </c>
       <c r="O112" t="n">
-        <v>-43.37</v>
+        <v>-46.12</v>
       </c>
       <c r="P112" t="n">
-        <v>-37.03</v>
+        <v>-36.99</v>
       </c>
       <c r="Q112" t="n">
-        <v>-22.37</v>
+        <v>-19.18</v>
       </c>
       <c r="R112" t="n">
-        <v>6.15</v>
+        <v>5.96</v>
       </c>
       <c r="S112" t="n">
-        <v>-30.57</v>
+        <v>-30.67</v>
       </c>
       <c r="T112" t="n">
-        <v>-4.59</v>
+        <v>-4.31</v>
       </c>
       <c r="U112" t="n">
-        <v>-1.3</v>
+        <v>-3.7</v>
       </c>
       <c r="V112" t="n">
-        <v>-0.91</v>
+        <v>-4.56</v>
       </c>
       <c r="W112" t="n">
-        <v>-37.02</v>
+        <v>-37.95</v>
       </c>
       <c r="X112" t="n">
-        <v>28.99</v>
+        <v>28.91</v>
       </c>
       <c r="Y112" t="n">
-        <v>81.47</v>
+        <v>81.3</v>
       </c>
       <c r="Z112" t="n">
         <v>-70.2</v>
       </c>
       <c r="AA112" t="n">
-        <v>-16.24</v>
+        <v>-18.63</v>
       </c>
       <c r="AB112" t="n">
-        <v>2.13</v>
+        <v>-4.44</v>
       </c>
       <c r="AC112" t="n">
-        <v>-63.02</v>
+        <v>-62.62</v>
       </c>
       <c r="AD112" t="n">
-        <v>-3.35</v>
+        <v>-0.39</v>
       </c>
       <c r="AE112" t="n">
-        <v>140.91</v>
+        <v>140.1</v>
       </c>
       <c r="AF112" t="n">
-        <v>-4.85</v>
+        <v>-7.47</v>
       </c>
       <c r="AG112" t="n">
-        <v>-3.6</v>
+        <v>-4.77</v>
       </c>
       <c r="AH112" t="n">
-        <v>13.06</v>
+        <v>12.85</v>
       </c>
       <c r="AI112" t="n">
-        <v>69.28</v>
+        <v>78.14</v>
       </c>
       <c r="AJ112" t="n">
-        <v>-16.99</v>
+        <v>-16.31</v>
       </c>
       <c r="AK112" t="n">
-        <v>-20.35</v>
+        <v>-22.09</v>
       </c>
       <c r="AL112" t="n">
-        <v>-21.8</v>
+        <v>-22.23</v>
       </c>
       <c r="AM112" t="n">
-        <v>-1.41</v>
+        <v>64.2</v>
       </c>
       <c r="AN112" t="n">
-        <v>2.29</v>
+        <v>-1.6</v>
       </c>
       <c r="AO112" t="n">
-        <v>-21.78</v>
+        <v>-21.84</v>
       </c>
       <c r="AP112" t="n">
-        <v>2.19</v>
+        <v>-0.4</v>
       </c>
       <c r="AQ112" t="n">
-        <v>-10.93</v>
+        <v>-14.92</v>
       </c>
       <c r="AR112" t="n">
-        <v>-2.29</v>
+        <v>-3.42</v>
       </c>
       <c r="AS112" t="n">
-        <v>11.82</v>
+        <v>3.21</v>
       </c>
       <c r="AT112" t="n">
-        <v>13.12</v>
+        <v>0.56</v>
       </c>
       <c r="AU112" t="n">
-        <v>-5.46</v>
+        <v>-7.53</v>
       </c>
       <c r="AV112" t="n">
-        <v>-34.51</v>
+        <v>-36.14</v>
       </c>
       <c r="AW112" t="n">
-        <v>-19.86</v>
+        <v>-20.26</v>
       </c>
       <c r="AX112" t="n">
-        <v>-32.94</v>
+        <v>-36.82</v>
       </c>
       <c r="AY112" t="n">
-        <v>-13.12</v>
+        <v>-16.54</v>
       </c>
       <c r="AZ112" t="n">
-        <v>-5.86</v>
+        <v>-3.55</v>
       </c>
       <c r="BA112" t="n">
-        <v>14.11</v>
+        <v>11.55</v>
       </c>
       <c r="BB112" t="n">
-        <v>5.81</v>
+        <v>6.65</v>
       </c>
       <c r="BC112" t="n">
-        <v>24.33</v>
+        <v>19.16</v>
       </c>
       <c r="BD112" t="n">
-        <v>80.09</v>
+        <v>204.13</v>
       </c>
       <c r="BE112" t="n">
-        <v>-25.32</v>
+        <v>-26.91</v>
       </c>
       <c r="BF112" t="n">
-        <v>-16.63</v>
+        <v>-18.21</v>
       </c>
       <c r="BG112" t="n">
-        <v>20.7</v>
+        <v>15.88</v>
       </c>
       <c r="BH112" t="n">
-        <v>-20.92</v>
+        <v>-14.63</v>
       </c>
       <c r="BI112" t="n">
-        <v>21.55</v>
+        <v>33.55</v>
       </c>
       <c r="BJ112" t="n">
-        <v>-2.93</v>
+        <v>-3.02</v>
       </c>
       <c r="BK112" t="n">
-        <v>2.44</v>
+        <v>2.49</v>
       </c>
       <c r="BL112" t="n">
-        <v>0.63</v>
+        <v>0.41</v>
       </c>
       <c r="BM112" t="n">
-        <v>0.35</v>
+        <v>0.62</v>
       </c>
       <c r="BN112" t="n">
-        <v>0.35</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="113">
@@ -54941,37 +55251,37 @@
         <v>45505</v>
       </c>
       <c r="B117" t="n">
-        <v>19.72</v>
+        <v>19.64</v>
       </c>
       <c r="C117" t="n">
-        <v>-0.9</v>
+        <v>-1.46</v>
       </c>
       <c r="D117" t="n">
-        <v>-3.11</v>
+        <v>1.93</v>
       </c>
       <c r="E117" t="n">
-        <v>11.24</v>
+        <v>7.64</v>
       </c>
       <c r="F117" t="n">
-        <v>3.03</v>
+        <v>2.12</v>
       </c>
       <c r="G117" t="n">
-        <v>27.8</v>
+        <v>30.79</v>
       </c>
       <c r="H117" t="n">
-        <v>37.36</v>
+        <v>38.11</v>
       </c>
       <c r="I117" t="n">
-        <v>-9.21</v>
+        <v>-8.61</v>
       </c>
       <c r="J117" t="n">
-        <v>-5.72</v>
+        <v>-6.61</v>
       </c>
       <c r="K117" t="n">
-        <v>21.5</v>
+        <v>21.48</v>
       </c>
       <c r="L117" t="n">
-        <v>30.46</v>
+        <v>30.39</v>
       </c>
       <c r="M117" t="n">
         <v>647.38</v>
@@ -54980,160 +55290,360 @@
         <v>-29.27</v>
       </c>
       <c r="O117" t="n">
-        <v>-78.93</v>
+        <v>-79.1</v>
       </c>
       <c r="P117" t="n">
-        <v>2.19</v>
+        <v>2.05</v>
       </c>
       <c r="Q117" t="n">
-        <v>11.28</v>
+        <v>11.05</v>
       </c>
       <c r="R117" t="n">
         <v>47.26</v>
       </c>
       <c r="S117" t="n">
-        <v>-15.04</v>
+        <v>-14.56</v>
       </c>
       <c r="T117" t="n">
-        <v>43.73</v>
+        <v>40.74</v>
       </c>
       <c r="U117" t="n">
-        <v>6.57</v>
+        <v>40.54</v>
       </c>
       <c r="V117" t="n">
-        <v>5.64</v>
+        <v>5.1</v>
       </c>
       <c r="W117" t="n">
-        <v>-12.26</v>
+        <v>-16.75</v>
       </c>
       <c r="X117" t="n">
-        <v>-7.07</v>
+        <v>-8.16</v>
       </c>
       <c r="Y117" t="n">
-        <v>26.55</v>
+        <v>25.04</v>
       </c>
       <c r="Z117" t="n">
         <v>-65.86</v>
       </c>
       <c r="AA117" t="n">
-        <v>13.47</v>
+        <v>15.09</v>
       </c>
       <c r="AB117" t="n">
-        <v>21.59</v>
+        <v>26.9</v>
       </c>
       <c r="AC117" t="n">
-        <v>-91.39</v>
+        <v>-91.5</v>
       </c>
       <c r="AD117" t="n">
         <v>-9.54</v>
       </c>
       <c r="AE117" t="n">
-        <v>-89.18</v>
+        <v>-88.57</v>
       </c>
       <c r="AF117" t="n">
-        <v>14.45</v>
+        <v>13.94</v>
       </c>
       <c r="AG117" t="n">
-        <v>19.93</v>
+        <v>19.49</v>
       </c>
       <c r="AH117" t="n">
-        <v>22.83</v>
+        <v>22.78</v>
       </c>
       <c r="AI117" t="n">
-        <v>87.29</v>
+        <v>87.85</v>
       </c>
       <c r="AJ117" t="n">
-        <v>10.3</v>
+        <v>7.93</v>
       </c>
       <c r="AK117" t="n">
-        <v>-19.48</v>
+        <v>-19.28</v>
       </c>
       <c r="AL117" t="n">
         <v>-5.31</v>
       </c>
       <c r="AM117" t="n">
-        <v>7.21</v>
+        <v>7.77</v>
       </c>
       <c r="AN117" t="n">
-        <v>-9.05</v>
+        <v>-9.77</v>
       </c>
       <c r="AO117" t="n">
-        <v>-15.3</v>
+        <v>-17.13</v>
       </c>
       <c r="AP117" t="n">
-        <v>-6.87</v>
+        <v>-9.33</v>
       </c>
       <c r="AQ117" t="n">
-        <v>25.32</v>
+        <v>24.87</v>
       </c>
       <c r="AR117" t="n">
-        <v>-2.14</v>
+        <v>-1.77</v>
       </c>
       <c r="AS117" t="n">
-        <v>24.29</v>
+        <v>23.51</v>
       </c>
       <c r="AT117" t="n">
-        <v>-18.72</v>
+        <v>-20.58</v>
       </c>
       <c r="AU117" t="n">
-        <v>1.53</v>
+        <v>2.36</v>
       </c>
       <c r="AV117" t="n">
-        <v>-23.95</v>
+        <v>-26.63</v>
       </c>
       <c r="AW117" t="n">
-        <v>45.88</v>
+        <v>45.95</v>
       </c>
       <c r="AX117" t="n">
-        <v>-23.6</v>
+        <v>-27.22</v>
       </c>
       <c r="AY117" t="n">
-        <v>28.83</v>
+        <v>28.56</v>
       </c>
       <c r="AZ117" t="n">
-        <v>11.25</v>
+        <v>10.67</v>
       </c>
       <c r="BA117" t="n">
-        <v>0.57</v>
+        <v>-1.03</v>
       </c>
       <c r="BB117" t="n">
-        <v>64.49</v>
+        <v>63.94</v>
       </c>
       <c r="BC117" t="n">
-        <v>1.35</v>
+        <v>0.58</v>
       </c>
       <c r="BD117" t="n">
-        <v>-64.36</v>
+        <v>-64.33</v>
       </c>
       <c r="BE117" t="n">
-        <v>18.34</v>
+        <v>15.87</v>
       </c>
       <c r="BF117" t="n">
-        <v>1.48</v>
+        <v>2.32</v>
       </c>
       <c r="BG117" t="n">
-        <v>-7.93</v>
+        <v>-8.18</v>
       </c>
       <c r="BH117" t="n">
-        <v>-8.66</v>
+        <v>-8.76</v>
       </c>
       <c r="BI117" t="n">
-        <v>37.09</v>
+        <v>38.15</v>
       </c>
       <c r="BJ117" t="n">
-        <v>19.16</v>
+        <v>18.96</v>
       </c>
       <c r="BK117" t="n">
         <v>-7.78</v>
       </c>
       <c r="BL117" t="n">
-        <v>-4.16</v>
+        <v>-4.41</v>
       </c>
       <c r="BM117" t="n">
-        <v>-73.64</v>
+        <v>-73.99</v>
       </c>
       <c r="BN117" t="n">
-        <v>-73.64</v>
+        <v>-73.99</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-35.85</v>
+      </c>
+      <c r="C118" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="D118" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-10.03</v>
+      </c>
+      <c r="F118" t="n">
+        <v>15.77</v>
+      </c>
+      <c r="G118" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H118" t="n">
+        <v>11.14</v>
+      </c>
+      <c r="I118" t="n">
+        <v>27.47</v>
+      </c>
+      <c r="J118" t="n">
+        <v>16.66</v>
+      </c>
+      <c r="K118" t="n">
+        <v>14.07</v>
+      </c>
+      <c r="L118" t="n">
+        <v>30.04</v>
+      </c>
+      <c r="M118" t="n">
+        <v>300.21</v>
+      </c>
+      <c r="N118" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="O118" t="n">
+        <v>-91.93</v>
+      </c>
+      <c r="P118" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>16.44</v>
+      </c>
+      <c r="R118" t="n">
+        <v>19.61</v>
+      </c>
+      <c r="S118" t="n">
+        <v>-26.88</v>
+      </c>
+      <c r="T118" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="U118" t="n">
+        <v>81.76</v>
+      </c>
+      <c r="V118" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="W118" t="n">
+        <v>-9.2</v>
+      </c>
+      <c r="X118" t="n">
+        <v>56.22</v>
+      </c>
+      <c r="Y118" t="n">
+        <v>-9.72</v>
+      </c>
+      <c r="Z118" t="n">
+        <v>-44.65</v>
+      </c>
+      <c r="AA118" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="AB118" t="n">
+        <v>10.66</v>
+      </c>
+      <c r="AC118" t="n">
+        <v>-91.18</v>
+      </c>
+      <c r="AD118" t="n">
+        <v>39.67</v>
+      </c>
+      <c r="AE118" t="n">
+        <v>-82.04</v>
+      </c>
+      <c r="AF118" t="n">
+        <v>-15.47</v>
+      </c>
+      <c r="AG118" t="n">
+        <v>77.36</v>
+      </c>
+      <c r="AH118" t="n">
+        <v>17.17</v>
+      </c>
+      <c r="AI118" t="n">
+        <v>98.07</v>
+      </c>
+      <c r="AJ118" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="AK118" t="n">
+        <v>-2.23</v>
+      </c>
+      <c r="AL118" t="n">
+        <v>-13.22</v>
+      </c>
+      <c r="AM118" t="n">
+        <v>35.01</v>
+      </c>
+      <c r="AN118" t="n">
+        <v>-7.11</v>
+      </c>
+      <c r="AO118" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AP118" t="n">
+        <v>12.44</v>
+      </c>
+      <c r="AQ118" t="n">
+        <v>17.23</v>
+      </c>
+      <c r="AR118" t="n">
+        <v>-6.41</v>
+      </c>
+      <c r="AS118" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AT118" t="n">
+        <v>20.32</v>
+      </c>
+      <c r="AU118" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="AV118" t="n">
+        <v>-38.77</v>
+      </c>
+      <c r="AW118" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="AX118" t="n">
+        <v>-25.51</v>
+      </c>
+      <c r="AY118" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AZ118" t="n">
+        <v>20.02</v>
+      </c>
+      <c r="BA118" t="n">
+        <v>-5.04</v>
+      </c>
+      <c r="BB118" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="BC118" t="n">
+        <v>14.27</v>
+      </c>
+      <c r="BD118" t="n">
+        <v>-5.73</v>
+      </c>
+      <c r="BE118" t="n">
+        <v>-5.8</v>
+      </c>
+      <c r="BF118" t="n">
+        <v>-9.58</v>
+      </c>
+      <c r="BG118" t="n">
+        <v>-30.49</v>
+      </c>
+      <c r="BH118" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="BI118" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="BJ118" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="BK118" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="BL118" t="n">
+        <v>19.83</v>
+      </c>
+      <c r="BM118" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="BN118" t="n">
+        <v>6.64</v>
       </c>
     </row>
   </sheetData>
@@ -57401,7 +57911,7 @@
         <v>-0.45</v>
       </c>
       <c r="G98" t="n">
-        <v>4.15</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="99">
@@ -57432,22 +57942,22 @@
         <v>45352</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.45</v>
+        <v>-0.46</v>
       </c>
       <c r="C100" t="n">
-        <v>0.29</v>
+        <v>0.33</v>
       </c>
       <c r="D100" t="n">
-        <v>-1.21</v>
+        <v>-1.17</v>
       </c>
       <c r="E100" t="n">
-        <v>-0.64</v>
+        <v>-0.69</v>
       </c>
       <c r="F100" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="G100" t="n">
-        <v>1.53</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="101">
@@ -57547,22 +58057,45 @@
         <v>45505</v>
       </c>
       <c r="B105" t="n">
-        <v>0.56</v>
+        <v>0.65</v>
       </c>
       <c r="C105" t="n">
-        <v>2.49</v>
+        <v>2.47</v>
       </c>
       <c r="D105" t="n">
-        <v>7.16</v>
+        <v>6.97</v>
       </c>
       <c r="E105" t="n">
-        <v>0.53</v>
+        <v>0.48</v>
       </c>
       <c r="F105" t="n">
-        <v>-0.2</v>
+        <v>-0.21</v>
       </c>
       <c r="G105" t="n">
-        <v>-3.05</v>
+        <v>-2.94</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="D106" t="n">
+        <v>35.91</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>